<commit_message>
fix(main): correct solve_tsp parameter in problem three
Changed full_coords to coords_q2 in solve_tsp call for problem three to use correct coordinates
</commit_message>
<xml_diff>
--- a/建模赛题附表数据.xlsx
+++ b/建模赛题附表数据.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sheldon/Documents/github_projects/express-route-opt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FBDED3-D6E5-9345-8E55-A31D515C0B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB7A93B-7B63-F949-B578-850F48B25B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11360" yWindow="6220" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16460" yWindow="2600" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="附表1_坐标" sheetId="1" r:id="rId1"/>
@@ -82,10 +82,11 @@
     <t>成本比例</t>
   </si>
   <si>
-    <t>货物量（吨）</t>
+    <t>编号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>编号</t>
+    <t>货物量（吨）</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -463,13 +464,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -645,7 +648,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="116" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
@@ -747,7 +752,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
@@ -1982,7 +1989,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
@@ -1991,7 +2000,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2">

</xml_diff>